<commit_message>
modif du excel ajout de d'heure de travail
</commit_message>
<xml_diff>
--- a/estimationFrédéricCôté.xlsx
+++ b/estimationFrédéricCôté.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4116" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4116" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Semaine 15</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t>Le projet doit être décomposé en plusieurs sections indépendantes qui doivent être priorisées et estimées</t>
   </si>
   <si>
@@ -174,6 +171,18 @@
   </si>
   <si>
     <t>modification barre de vie et ajout des kill et fonction de leveling</t>
+  </si>
+  <si>
+    <t>ajout d'un système d'achat de skill</t>
+  </si>
+  <si>
+    <t>ajout d'une classe joueur</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2017-03-02</t>
+  </si>
+  <si>
+    <t>ajout d'une fonction de critique</t>
   </si>
 </sst>
 </file>
@@ -317,7 +326,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -370,6 +379,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1639,7 +1649,7 @@
   <sheetData>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1684,7 +1694,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="3">
         <v>15</v>
@@ -1695,7 +1705,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3">
         <v>25</v>
@@ -1706,7 +1716,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C18" s="3">
         <v>10</v>
@@ -1717,7 +1727,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C19" s="3">
         <v>15</v>
@@ -1728,7 +1738,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C20" s="3">
         <v>5</v>
@@ -1772,7 +1782,7 @@
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="3">
         <v>5</v>
@@ -1783,7 +1793,7 @@
         <v>2</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="3">
         <v>5</v>
@@ -1794,7 +1804,7 @@
         <v>3</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="3">
         <v>10</v>
@@ -1866,7 +1876,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
@@ -1928,7 +1938,7 @@
         <v>42765</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
@@ -1939,7 +1949,7 @@
         <v>42766</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="15">
         <v>2</v>
@@ -1950,7 +1960,7 @@
         <v>42772</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="15">
         <v>3</v>
@@ -1961,7 +1971,7 @@
         <v>42773</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="15">
         <v>2</v>
@@ -1972,7 +1982,7 @@
         <v>42774</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="15">
         <v>2</v>
@@ -1983,7 +1993,7 @@
         <v>42779</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="15">
         <v>3</v>
@@ -1994,7 +2004,7 @@
         <v>42780</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="15">
         <v>2</v>
@@ -2005,7 +2015,7 @@
         <v>42782</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21" s="15">
         <v>2</v>
@@ -2016,7 +2026,7 @@
         <v>42783</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="15">
         <v>1</v>
@@ -2104,13 +2114,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2119,7 +2129,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="21"/>
     </row>
@@ -2153,8 +2163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,28 +2225,44 @@
         <v>42786</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C14" s="15">
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
+      <c r="A15" s="24">
+        <v>42788</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
+      <c r="A16" s="24">
+        <v>42789</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="15">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
+        <v>53</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="15">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
@@ -2340,18 +2366,18 @@
       <c r="B37" s="20"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2360,7 +2386,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="21"/>
     </row>
@@ -2578,13 +2604,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2593,7 +2619,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="21"/>
     </row>
@@ -2664,7 +2690,7 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2811,13 +2837,13 @@
     </row>
     <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
@@ -2826,7 +2852,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="21"/>
     </row>

</xml_diff>

<commit_message>
itération 3 ajout d'auto-évaluation
</commit_message>
<xml_diff>
--- a/estimationFrédéricCôté.xlsx
+++ b/estimationFrédéricCôté.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>ajout de cla classe marcher et réfléchir sur l'utilisation de celle-ci</t>
+  </si>
+  <si>
+    <t>pas ma meilleur itération à date j'ai l'impression d'aucunement avancé</t>
   </si>
 </sst>
 </file>
@@ -2518,8 +2521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2758,7 +2761,9 @@
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="4"/>
+      <c r="B40" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
@@ -2767,7 +2772,9 @@
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="22"/>
+      <c r="B42" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="23"/>

</xml_diff>

<commit_message>
itération 4 final excel
</commit_message>
<xml_diff>
--- a/estimationFrédéricCôté.xlsx
+++ b/estimationFrédéricCôté.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18067"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4116" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="4110" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Estimation" sheetId="1" r:id="rId1"/>
@@ -13,12 +13,12 @@
     <sheet name="Iteration #3" sheetId="4" r:id="rId4"/>
     <sheet name="Iteration #4" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="85">
   <si>
     <t>Définition du noyau (section qui doit obligatoirement être terminée pour réussir le cours : 60%)</t>
   </si>
@@ -234,12 +234,51 @@
   </si>
   <si>
     <t>pas ma meilleur itération à date j'ai l'impression d'aucunement avancé</t>
+  </si>
+  <si>
+    <t>ajout de son boom de mort et création de d'icon</t>
+  </si>
+  <si>
+    <t>ajout d'image de background modification</t>
+  </si>
+  <si>
+    <t>ajout de la view du marché</t>
+  </si>
+  <si>
+    <t>travail de création de monstre</t>
+  </si>
+  <si>
+    <t>création d'un deuxieme monstre</t>
+  </si>
+  <si>
+    <t>ajout de la nouvelle monnaie pour acheter des chose dans le market avec fonction de calcule</t>
+  </si>
+  <si>
+    <t>changement de fonctionnement de variable dans un object</t>
+  </si>
+  <si>
+    <t>modification mineur et optimisation des fonction de calcule pour stopper les erreurs</t>
+  </si>
+  <si>
+    <t>ajout des bouton du market avec prix et % d'augmentation</t>
+  </si>
+  <si>
+    <t>tentative de recupérer les donner perdu en changement de view</t>
+  </si>
+  <si>
+    <t>power points</t>
+  </si>
+  <si>
+    <t>présentation oral</t>
+  </si>
+  <si>
+    <t>c'est malheureusement pas ma meilleur itération malgré beaucoup d'heure je semblais ne pas avancer le travail de modification des graphisme prenais beaucoup de temps.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -377,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -431,6 +470,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,7 +507,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="Rectangle 2"/>
+        <xdr:cNvPr id="1026" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -527,7 +575,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="ZoneTexte 2"/>
+        <xdr:cNvPr id="3" name="ZoneTexte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -587,7 +641,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Image 1" descr="dicj1"/>
+        <xdr:cNvPr id="2" name="Image 1" descr="dicj1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -655,7 +715,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="Rectangle 2"/>
+        <xdr:cNvPr id="5" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -717,7 +783,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="ZoneTexte 5"/>
+        <xdr:cNvPr id="6" name="ZoneTexte 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -777,7 +849,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="7" name="Image 6" descr="dicj1"/>
+        <xdr:cNvPr id="7" name="Image 6" descr="dicj1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -845,7 +923,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 2"/>
+        <xdr:cNvPr id="2" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -907,7 +991,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="ZoneTexte 2"/>
+        <xdr:cNvPr id="3" name="ZoneTexte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -967,7 +1057,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3" descr="dicj1"/>
+        <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1035,7 +1131,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 2"/>
+        <xdr:cNvPr id="2" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1097,7 +1199,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="ZoneTexte 2"/>
+        <xdr:cNvPr id="3" name="ZoneTexte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1157,7 +1265,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3" descr="dicj1"/>
+        <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1225,7 +1339,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Rectangle 2"/>
+        <xdr:cNvPr id="2" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1287,7 +1407,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="ZoneTexte 2"/>
+        <xdr:cNvPr id="3" name="ZoneTexte 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -1347,7 +1473,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Image 3" descr="dicj1"/>
+        <xdr:cNvPr id="4" name="Image 3" descr="dicj1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -1474,6 +1606,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1509,6 +1658,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1691,45 +1857,45 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.44140625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.42578125" customWidth="1"/>
+    <col min="2" max="2" width="64.5703125" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="5.55" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="5.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1740,7 +1906,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="10">
         <v>1</v>
       </c>
@@ -1751,7 +1917,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="10">
         <v>2</v>
       </c>
@@ -1762,7 +1928,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1773,7 +1939,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>4</v>
       </c>
@@ -1784,7 +1950,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>5</v>
       </c>
@@ -1795,7 +1961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>9</v>
       </c>
@@ -1805,19 +1971,19 @@
         <v>70</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C23" s="1"/>
     </row>
-    <row r="24" spans="1:3" ht="5.55" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" ht="5.65" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>4</v>
       </c>
@@ -1828,7 +1994,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="10">
         <v>1</v>
       </c>
@@ -1839,7 +2005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="10">
         <v>2</v>
       </c>
@@ -1850,7 +2016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="10">
         <v>3</v>
       </c>
@@ -1861,42 +2027,42 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="10">
         <v>4</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="10">
         <v>5</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="10">
         <v>6</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="10">
         <v>7</v>
       </c>
       <c r="B32" s="4"/>
       <c r="C32" s="3"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="10">
         <v>8</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="3"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="20" t="s">
         <v>9</v>
       </c>
@@ -1906,7 +2072,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="str">
         <f>IF(C21+C34&lt;90,"Il manque "&amp;90-(C21+C34)&amp;"h",IF(C21+C34&gt;90,"Il y a "&amp;(C21+C34)-90&amp;"h de trop",""))</f>
         <v/>
@@ -1931,19 +2097,19 @@
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -1951,7 +2117,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1959,7 +2125,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -1967,13 +2133,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.55" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -1984,7 +2150,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42765</v>
       </c>
@@ -1995,7 +2161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="18">
         <v>42766</v>
       </c>
@@ -2006,7 +2172,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="18">
         <v>42772</v>
       </c>
@@ -2017,7 +2183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <v>42773</v>
       </c>
@@ -2028,7 +2194,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>42774</v>
       </c>
@@ -2039,7 +2205,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="18">
         <v>42779</v>
       </c>
@@ -2050,7 +2216,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="18">
         <v>42780</v>
       </c>
@@ -2061,7 +2227,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="18">
         <v>42782</v>
       </c>
@@ -2072,7 +2238,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="18">
         <v>42783</v>
       </c>
@@ -2083,77 +2249,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
@@ -2163,40 +2329,40 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
       <c r="B40" s="4"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="23"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="23"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="23"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
     </row>
   </sheetData>
@@ -2218,19 +2384,19 @@
       <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2238,7 +2404,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2246,7 +2412,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2254,13 +2420,13 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.55" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2271,7 +2437,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42786</v>
       </c>
@@ -2282,7 +2448,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>42788</v>
       </c>
@@ -2293,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>42789</v>
       </c>
@@ -2304,7 +2470,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>53</v>
       </c>
@@ -2315,7 +2481,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>42800</v>
       </c>
@@ -2326,7 +2492,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>42800</v>
       </c>
@@ -2337,7 +2503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>42802</v>
       </c>
@@ -2348,7 +2514,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>42802</v>
       </c>
@@ -2359,7 +2525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>42807</v>
       </c>
@@ -2370,7 +2536,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="19">
         <v>42807</v>
       </c>
@@ -2381,7 +2547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="19">
         <v>42809</v>
       </c>
@@ -2392,7 +2558,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>42812</v>
       </c>
@@ -2403,62 +2569,62 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
@@ -2468,13 +2634,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2482,28 +2648,28 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
       <c r="B42" s="22"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="23"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="23"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="23"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
     </row>
   </sheetData>
@@ -2521,23 +2687,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B42" sqref="B42:B47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2545,7 +2711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2553,7 +2719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2561,13 +2727,13 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.55" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2578,7 +2744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="12">
         <v>42814</v>
       </c>
@@ -2589,7 +2755,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="19">
         <v>42815</v>
       </c>
@@ -2600,7 +2766,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="19">
         <v>42821</v>
       </c>
@@ -2611,7 +2777,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>42821</v>
       </c>
@@ -2622,7 +2788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="19">
         <v>42822</v>
       </c>
@@ -2633,7 +2799,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="19">
         <v>42828</v>
       </c>
@@ -2644,7 +2810,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>42829</v>
       </c>
@@ -2655,7 +2821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="19">
         <v>42831</v>
       </c>
@@ -2666,82 +2832,82 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="15"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="15"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="15"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="15"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="15"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
@@ -2751,13 +2917,13 @@
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
@@ -2765,10 +2931,10 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
@@ -2776,19 +2942,19 @@
         <v>71</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="23"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="23"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="23"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
     </row>
   </sheetData>
@@ -2806,23 +2972,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:C47"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" customWidth="1"/>
-    <col min="2" max="2" width="70.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="70.7109375" customWidth="1"/>
     <col min="3" max="3" width="9" style="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>11</v>
       </c>
@@ -2830,7 +2996,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -2838,7 +3004,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>13</v>
       </c>
@@ -2846,13 +3012,13 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="5.55" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="5.65" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>15</v>
       </c>
@@ -2863,165 +3029,247 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="12"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="15"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="15"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="15"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="15"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="15"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="15"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="15"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="15"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="15"/>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="15"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="15"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="12">
+        <v>42470</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="19">
+        <v>42471</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="19">
+        <v>42474</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
+        <v>42477</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="19">
+        <v>42478</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="19">
+        <v>42482</v>
+      </c>
+      <c r="B19" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="C19" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="19">
+        <v>42483</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="19">
+        <v>42489</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="19">
+        <v>42490</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="19">
+        <v>42491</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="19">
+        <v>42497</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C24" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19">
+        <v>42498</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="19">
+        <v>42499</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="15"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="15"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="15"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="15"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="15"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="15"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20" t="s">
         <v>9</v>
       </c>
       <c r="B37" s="21"/>
       <c r="C37" s="16">
         <f>SUM(C14:C36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C39" s="17"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="B40" s="4"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B42" s="22"/>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B43" s="23"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B44" s="23"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B45" s="23"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B46" s="23"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B47" s="24"/>
     </row>
   </sheetData>

</xml_diff>